<commit_message>
killer and prereq cells implemented and checked
</commit_message>
<xml_diff>
--- a/excel/MasterGalleryKey.xlsx
+++ b/excel/MasterGalleryKey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanfa/workspace/pysheetgrader/sample_excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandeepyadav/Desktop/Pysheetgrader/pysheetgrader-parent/pysheetgrader-core/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3DCD68-785F-6145-9329-0476F14CBB7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C944A9-D242-D946-9CC5-3FAEAFB68960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37320" yWindow="1320" windowWidth="19200" windowHeight="19440" firstSheet="1" activeTab="3" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="4440" yWindow="2680" windowWidth="28800" windowHeight="16460" firstSheet="2" activeTab="6" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -30,15 +30,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -1524,7 +1515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>Number</t>
   </si>
@@ -1683,6 +1674,12 @@
   </si>
   <si>
     <t>// student is correct 3003 = 1001 + 2002 = 4004 - 1001</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -2408,7 +2405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF2EB7E-182E-C148-9132-E2AAE2C42630}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -2600,7 +2597,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2705,15 +2702,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EABA77-C8A8-0247-A6AC-2452B8B329D1}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="213" zoomScaleNormal="213" workbookViewId="0">
-      <selection sqref="A1:B8"/>
+    <sheetView tabSelected="1" zoomScale="213" zoomScaleNormal="213" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2721,7 +2718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2729,7 +2726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2737,31 +2734,40 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2769,7 +2775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2908,15 +2914,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF83535-20BE-CA43-B82B-2F0E1F118D83}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="224" zoomScaleNormal="224" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2924,7 +2930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2935,7 +2941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2943,15 +2949,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2959,7 +2968,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2967,7 +2976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2975,7 +2984,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2983,7 +2992,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>

</xml_diff>